<commit_message>
mais alguns diagramas de sequencia
</commit_message>
<xml_diff>
--- a/Detalhes_Use_Cases.xlsx
+++ b/Detalhes_Use_Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arturleite/dev/DSS/DSS_TP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CE24FF-A11A-C24C-9953-250C312AB616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DCC806-43F0-EA4E-B39E-5745934FC78E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="12920" firstSheet="15" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="25600" windowHeight="12920" firstSheet="15" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEMPLATE" sheetId="2" r:id="rId1"/>
@@ -1810,9 +1810,6 @@
     <t>Começar Corrida</t>
   </si>
   <si>
-    <t>startRace(circuito: Circuito, situacao: Meteorologia)</t>
-  </si>
-  <si>
     <t>getRankingGlobal(): Tabela</t>
   </si>
   <si>
@@ -1865,6 +1862,9 @@
   </si>
   <si>
     <t>autenticaUser(username: String, password: String): User</t>
+  </si>
+  <si>
+    <t>startNextRace(): String</t>
   </si>
 </sst>
 </file>
@@ -2686,7 +2686,7 @@
         <v>265</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>270</v>
@@ -3489,7 +3489,7 @@
         <v>280</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>270</v>
@@ -3772,10 +3772,10 @@
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>318</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>319</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>256</v>
@@ -3882,7 +3882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="B1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="D3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -4031,10 +4031,10 @@
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>262</v>
@@ -4068,10 +4068,10 @@
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>321</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>322</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>258</v>
@@ -4329,7 +4329,7 @@
         <v>292</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4453,8 +4453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="B1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:H11"/>
+    <sheetView topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -4646,7 +4646,7 @@
         <v>312</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>313</v>
+        <v>331</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>311</v>
@@ -4958,7 +4958,7 @@
         <v>297</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>311</v>
@@ -4973,10 +4973,10 @@
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>311</v>
@@ -5556,10 +5556,10 @@
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>325</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>326</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>257</v>
@@ -5829,7 +5829,7 @@
         <v>267</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5938,7 +5938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="B1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="D2" zoomScaleNormal="69" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScaleNormal="69" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -6075,7 +6075,7 @@
         <v>268</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6093,7 +6093,7 @@
         <v>267</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6105,10 +6105,10 @@
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>329</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>330</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>270</v>
@@ -6252,7 +6252,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="B1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:F8"/>
     </sheetView>
   </sheetViews>
@@ -6411,7 +6411,7 @@
         <v>271</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>270</v>
@@ -6745,7 +6745,7 @@
         <v>303</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>257</v>

</xml_diff>